<commit_message>
Adding the messages to the Excel spreadsheet.
</commit_message>
<xml_diff>
--- a/dpub-aria-testing/test-results/DPUB-ARIA-suggested-output.xlsx
+++ b/dpub-aria-testing/test-results/DPUB-ARIA-suggested-output.xlsx
@@ -1,16 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23801"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D653250F-EDC1-794F-8C2D-98A314D2ACD2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C9ED60E-B346-4528-963E-A95D7151212C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="840" windowWidth="28200" windowHeight="17160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="results" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
+    <definedName name="Title_2fa3e308fb9b491582d3067559beb00c" localSheetId="0">results!$A$1</definedName>
     <definedName name="Title_8e133929154a42a88c65db5298a3d721" localSheetId="0">results!#REF!</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
@@ -18,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="79">
   <si>
     <t>doc-abstract</t>
   </si>
@@ -147,6 +148,114 @@
   </si>
   <si>
     <t>Placement (pre/post)</t>
+  </si>
+  <si>
+    <t>abstract</t>
+  </si>
+  <si>
+    <t>acknowledgements</t>
+  </si>
+  <si>
+    <t>afterward</t>
+  </si>
+  <si>
+    <t>appendix</t>
+  </si>
+  <si>
+    <t>bibliography</t>
+  </si>
+  <si>
+    <t>chapter</t>
+  </si>
+  <si>
+    <t>conclusion</t>
+  </si>
+  <si>
+    <t>cover</t>
+  </si>
+  <si>
+    <t>credits</t>
+  </si>
+  <si>
+    <t>credit</t>
+  </si>
+  <si>
+    <t>dedication</t>
+  </si>
+  <si>
+    <t>end notes</t>
+  </si>
+  <si>
+    <t>epigraph</t>
+  </si>
+  <si>
+    <t>epilogue</t>
+  </si>
+  <si>
+    <t>errata</t>
+  </si>
+  <si>
+    <t>example</t>
+  </si>
+  <si>
+    <t>footnote</t>
+  </si>
+  <si>
+    <t>forward</t>
+  </si>
+  <si>
+    <t>Table of Contents</t>
+  </si>
+  <si>
+    <t>tip</t>
+  </si>
+  <si>
+    <t>subtitle</t>
+  </si>
+  <si>
+    <t>question and answer</t>
+  </si>
+  <si>
+    <t>prologue</t>
+  </si>
+  <si>
+    <t>preface</t>
+  </si>
+  <si>
+    <t>part</t>
+  </si>
+  <si>
+    <t>list of pages</t>
+  </si>
+  <si>
+    <t>page break</t>
+  </si>
+  <si>
+    <t>notice</t>
+  </si>
+  <si>
+    <t>introduction</t>
+  </si>
+  <si>
+    <t>index</t>
+  </si>
+  <si>
+    <t>reference to glossary term</t>
+  </si>
+  <si>
+    <t>colophon</t>
+  </si>
+  <si>
+    <t>back to referencing item</t>
+  </si>
+  <si>
+    <t>reference to note item</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> emphasized quote</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> reference to bibliographic entry</t>
   </si>
 </sst>
 </file>
@@ -539,34 +648,34 @@
   <dimension ref="A1:D40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B26" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D2" sqref="D2"/>
+      <selection pane="bottomRight" activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="49.83203125" customWidth="1"/>
-    <col min="3" max="3" width="17.6640625" customWidth="1"/>
-    <col min="4" max="4" width="22.33203125" customWidth="1"/>
-    <col min="5" max="5" width="9.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.83203125" customWidth="1"/>
-    <col min="7" max="7" width="15.5" customWidth="1"/>
-    <col min="8" max="8" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.33203125" customWidth="1"/>
-    <col min="11" max="11" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18.5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.36328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="49.81640625" customWidth="1"/>
+    <col min="3" max="3" width="17.6328125" customWidth="1"/>
+    <col min="4" max="4" width="22.36328125" customWidth="1"/>
+    <col min="5" max="5" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.81640625" customWidth="1"/>
+    <col min="7" max="7" width="15.453125" customWidth="1"/>
+    <col min="8" max="8" width="9.6328125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.36328125" customWidth="1"/>
+    <col min="11" max="11" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.453125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.6328125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.36328125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.6328125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="15" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="27.6640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="27.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>39</v>
       </c>
@@ -580,197 +689,308 @@
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B10" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B11" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B12" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B13" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B14" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B15" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B16" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B17" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B18" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B19" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B20" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B21" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B22" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B24" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B25" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B26" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B27" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B28" t="s">
+        <v>70</v>
+      </c>
+      <c r="C28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B29" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B30" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B31" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B32" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B33" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B34" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B35" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B36" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B37" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B38" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>38</v>
       </c>

</xml_diff>

<commit_message>
Added the priority to the list of messages. Also added some comments.
</commit_message>
<xml_diff>
--- a/dpub-aria-testing/test-results/DPUB-ARIA-suggested-output.xlsx
+++ b/dpub-aria-testing/test-results/DPUB-ARIA-suggested-output.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23901"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C425F49-2457-2A4E-A8C1-42151D0121A1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19CBFDEE-C804-4B52-8ECA-342821903366}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="results" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="90">
   <si>
     <t>doc-abstract</t>
   </si>
@@ -259,6 +259,36 @@
   </si>
   <si>
     <t>reference to bibliographic entry</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>Medium</t>
+  </si>
+  <si>
+    <t>With the priority, we are putting in High, medium, and low. We mean a high priority would always be presented, so even if a verbosity setting was set to low, it would still be presented.</t>
+  </si>
+  <si>
+    <t>High</t>
+  </si>
+  <si>
+    <t>Low</t>
+  </si>
+  <si>
+    <t>Normally this would be placed on the section element before the H1 or h2 that follows it. The announcement would be better than the generic "landmark".</t>
+  </si>
+  <si>
+    <t>We think that this may appear on each example, which could become too tedious.</t>
+  </si>
+  <si>
+    <t>We felt letting people that the link was to a specific type of element would be good.</t>
+  </si>
+  <si>
+    <t>Notices are many times cautions, posion, warnings, which should always be presented.</t>
+  </si>
+  <si>
+    <t>This would let the reader know they were going back to the referencing item.</t>
   </si>
 </sst>
 </file>
@@ -648,37 +678,37 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D40"/>
+  <dimension ref="A1:E40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="C31" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B9" sqref="B9"/>
+      <selection pane="bottomRight" activeCell="C46" sqref="C46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="49.83203125" customWidth="1"/>
-    <col min="3" max="3" width="17.6640625" customWidth="1"/>
-    <col min="4" max="4" width="22.33203125" customWidth="1"/>
-    <col min="5" max="5" width="9.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.83203125" customWidth="1"/>
-    <col min="7" max="7" width="15.5" customWidth="1"/>
-    <col min="8" max="8" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.33203125" customWidth="1"/>
-    <col min="11" max="11" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18.5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.36328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="49.81640625" customWidth="1"/>
+    <col min="3" max="3" width="17.6328125" customWidth="1"/>
+    <col min="4" max="4" width="22.36328125" customWidth="1"/>
+    <col min="5" max="5" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.81640625" customWidth="1"/>
+    <col min="7" max="7" width="15.453125" customWidth="1"/>
+    <col min="8" max="8" width="9.6328125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.36328125" customWidth="1"/>
+    <col min="11" max="11" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.453125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.6328125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.36328125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.6328125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="15" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="27.6640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="27.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>39</v>
       </c>
@@ -691,312 +721,441 @@
       <c r="D1" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C2" t="s">
+        <v>81</v>
+      </c>
+      <c r="E2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C3" t="s">
+        <v>81</v>
+      </c>
+      <c r="E3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>3</v>
       </c>
       <c r="B5" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>4</v>
       </c>
       <c r="B6" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C6" t="s">
+        <v>83</v>
+      </c>
+      <c r="E6" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>5</v>
       </c>
       <c r="B7" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C7" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>6</v>
       </c>
       <c r="B8" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C8" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>7</v>
       </c>
       <c r="B9" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C9" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>8</v>
       </c>
       <c r="B10" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C10" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>9</v>
       </c>
       <c r="B11" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C11" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>10</v>
       </c>
       <c r="B12" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C12" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>11</v>
       </c>
       <c r="B13" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C13" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>12</v>
       </c>
       <c r="B14" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C14" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>13</v>
       </c>
       <c r="B15" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C15" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>14</v>
       </c>
       <c r="B16" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C16" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>15</v>
       </c>
       <c r="B17" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C17" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>16</v>
       </c>
       <c r="B18" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C18" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>17</v>
       </c>
       <c r="B19" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C19" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>18</v>
       </c>
       <c r="B20" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C20" t="s">
+        <v>84</v>
+      </c>
+      <c r="E20" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>19</v>
       </c>
       <c r="B21" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C21" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>20</v>
       </c>
       <c r="B22" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C22" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>21</v>
       </c>
       <c r="B23" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C23" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>22</v>
       </c>
       <c r="B24" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C24" t="s">
+        <v>83</v>
+      </c>
+      <c r="E24" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>23</v>
       </c>
       <c r="B25" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C25" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>24</v>
       </c>
       <c r="B26" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C26" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>25</v>
       </c>
       <c r="B27" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C27" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>26</v>
       </c>
       <c r="B28" t="s">
         <v>70</v>
       </c>
-      <c r="C28">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C28" t="s">
+        <v>83</v>
+      </c>
+      <c r="E28" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>27</v>
       </c>
       <c r="B29" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C29" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>28</v>
       </c>
       <c r="B30" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C30" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>29</v>
       </c>
       <c r="B31" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C31" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>30</v>
       </c>
       <c r="B32" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C32" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>31</v>
       </c>
       <c r="B33" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C33" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>32</v>
       </c>
       <c r="B34" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C34" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>33</v>
       </c>
       <c r="B35" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C35" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>34</v>
       </c>
       <c r="B36" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C36" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>35</v>
       </c>
       <c r="B37" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C37" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>36</v>
       </c>
       <c r="B38" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C38" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>38</v>
       </c>

</xml_diff>

<commit_message>
Updates to recommended output after June 1 2021 call
</commit_message>
<xml_diff>
--- a/dpub-aria-testing/test-results/DPUB-ARIA-suggested-output.xlsx
+++ b/dpub-aria-testing/test-results/DPUB-ARIA-suggested-output.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24026"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19CBFDEE-C804-4B52-8ECA-342821903366}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{336BFA0B-C3DC-4649-BAFD-908E8B43EE8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -11,6 +11,7 @@
     <sheet name="results" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
+    <definedName name="_GoBack" localSheetId="0">results!$B$34</definedName>
     <definedName name="Title_2fa3e308fb9b491582d3067559beb00c" localSheetId="0">results!$A$1</definedName>
     <definedName name="Title_8e133929154a42a88c65db5298a3d721" localSheetId="0">results!#REF!</definedName>
   </definedNames>
@@ -240,27 +241,12 @@
     <t>index</t>
   </si>
   <si>
-    <t>reference to glossary term</t>
-  </si>
-  <si>
     <t>colophon</t>
   </si>
   <si>
-    <t>back to referencing item</t>
-  </si>
-  <si>
-    <t>reference to note item</t>
-  </si>
-  <si>
-    <t>emphasized quote</t>
-  </si>
-  <si>
     <t>glossary</t>
   </si>
   <si>
-    <t>reference to bibliographic entry</t>
-  </si>
-  <si>
     <t>Comments</t>
   </si>
   <si>
@@ -289,6 +275,21 @@
   </si>
   <si>
     <t>This would let the reader know they were going back to the referencing item.</t>
+  </si>
+  <si>
+    <t>backlink</t>
+  </si>
+  <si>
+    <t>Glossary reference</t>
+  </si>
+  <si>
+    <t>note reference</t>
+  </si>
+  <si>
+    <t>Emphasised Excerpt</t>
+  </si>
+  <si>
+    <t>Bibliographic reference</t>
   </si>
 </sst>
 </file>
@@ -332,13 +333,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -681,10 +685,10 @@
   <dimension ref="A1:E40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="C31" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B24" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C46" sqref="C46"/>
+      <selection pane="bottomRight" activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -722,7 +726,7 @@
         <v>42</v>
       </c>
       <c r="E1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
@@ -733,10 +737,10 @@
         <v>43</v>
       </c>
       <c r="C2" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="E2" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
@@ -747,10 +751,10 @@
         <v>44</v>
       </c>
       <c r="C3" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="E3" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
@@ -761,7 +765,7 @@
         <v>45</v>
       </c>
       <c r="C4" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
@@ -772,7 +776,7 @@
         <v>46</v>
       </c>
       <c r="C5" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
@@ -780,13 +784,13 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="C6" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="E6" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
@@ -797,18 +801,18 @@
         <v>47</v>
       </c>
       <c r="C7" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>6</v>
       </c>
-      <c r="B8" t="s">
-        <v>79</v>
+      <c r="B8" s="3" t="s">
+        <v>89</v>
       </c>
       <c r="C8" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
@@ -819,7 +823,7 @@
         <v>48</v>
       </c>
       <c r="C9" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
@@ -827,10 +831,10 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C10" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
@@ -841,7 +845,7 @@
         <v>49</v>
       </c>
       <c r="C11" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
@@ -852,7 +856,7 @@
         <v>50</v>
       </c>
       <c r="C12" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
@@ -863,7 +867,7 @@
         <v>52</v>
       </c>
       <c r="C13" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
@@ -874,7 +878,7 @@
         <v>51</v>
       </c>
       <c r="C14" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
@@ -885,7 +889,7 @@
         <v>53</v>
       </c>
       <c r="C15" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
@@ -896,7 +900,7 @@
         <v>54</v>
       </c>
       <c r="C16" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
@@ -907,7 +911,7 @@
         <v>55</v>
       </c>
       <c r="C17" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
@@ -918,7 +922,7 @@
         <v>56</v>
       </c>
       <c r="C18" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
@@ -929,7 +933,7 @@
         <v>57</v>
       </c>
       <c r="C19" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
@@ -940,10 +944,10 @@
         <v>58</v>
       </c>
       <c r="C20" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="E20" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
@@ -954,7 +958,7 @@
         <v>59</v>
       </c>
       <c r="C21" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
@@ -965,7 +969,7 @@
         <v>60</v>
       </c>
       <c r="C22" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
@@ -973,24 +977,24 @@
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="C23" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>22</v>
       </c>
-      <c r="B24" t="s">
-        <v>73</v>
+      <c r="B24" s="3" t="s">
+        <v>86</v>
       </c>
       <c r="C24" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="E24" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.35">
@@ -1001,7 +1005,7 @@
         <v>72</v>
       </c>
       <c r="C25" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.35">
@@ -1012,7 +1016,7 @@
         <v>71</v>
       </c>
       <c r="C26" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.35">
@@ -1020,10 +1024,10 @@
         <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>76</v>
+        <v>87</v>
       </c>
       <c r="C27" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.35">
@@ -1034,10 +1038,10 @@
         <v>70</v>
       </c>
       <c r="C28" t="s">
+        <v>78</v>
+      </c>
+      <c r="E28" t="s">
         <v>83</v>
-      </c>
-      <c r="E28" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.35">
@@ -1048,7 +1052,7 @@
         <v>69</v>
       </c>
       <c r="C29" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.35">
@@ -1059,7 +1063,7 @@
         <v>68</v>
       </c>
       <c r="C30" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.35">
@@ -1070,7 +1074,7 @@
         <v>67</v>
       </c>
       <c r="C31" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.35">
@@ -1081,7 +1085,7 @@
         <v>66</v>
       </c>
       <c r="C32" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.35">
@@ -1092,18 +1096,18 @@
         <v>65</v>
       </c>
       <c r="C33" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>32</v>
       </c>
-      <c r="B34" t="s">
-        <v>77</v>
+      <c r="B34" s="3" t="s">
+        <v>88</v>
       </c>
       <c r="C34" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.35">
@@ -1114,7 +1118,7 @@
         <v>64</v>
       </c>
       <c r="C35" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.35">
@@ -1125,7 +1129,7 @@
         <v>63</v>
       </c>
       <c r="C36" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.35">
@@ -1136,7 +1140,7 @@
         <v>62</v>
       </c>
       <c r="C37" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.35">
@@ -1147,7 +1151,7 @@
         <v>61</v>
       </c>
       <c r="C38" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.35">

</xml_diff>